<commit_message>
LESSON 16 - Database - 16.02.2025
</commit_message>
<xml_diff>
--- a/Java23 QuyenPhan Database Design.xlsx
+++ b/Java23 QuyenPhan Database Design.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java23\3. Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501E8FF5-C810-4696-8157-FAB85EDD4571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349C1669-8412-4DF6-B078-A6A01BE6D247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="588" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mô hình quan niệm" sheetId="1" r:id="rId1"/>
-    <sheet name="ERD - Mô hình logic" sheetId="2" r:id="rId2"/>
-    <sheet name="RD - Mô hình quan hệ" sheetId="3" r:id="rId3"/>
-    <sheet name="DB - Mô hình vật lý" sheetId="4" r:id="rId4"/>
+    <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
+    <sheet name="B2. Mô hình logic" sheetId="5" r:id="rId2"/>
+    <sheet name="ERD - Mô hình logic" sheetId="2" r:id="rId3"/>
+    <sheet name="RD - Mô hình quan hệ" sheetId="3" r:id="rId4"/>
+    <sheet name="DB - Mô hình vật lý" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,8 +28,76 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Quyen Ngoc Phan</author>
+  </authors>
+  <commentList>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{8361C4F5-FAEE-4C10-B5BB-5A2FF1D8C2C3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Lưu trữ cùng với kích cỡ, chất liệu, màu sắc</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Quyen Ngoc Phan</author>
+  </authors>
+  <commentList>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{F496D48F-A2BA-48FB-ACCA-2D383B7B2F89}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Lưu trữ cùng với kích cỡ, chất liệu, màu sắc</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="271">
   <si>
     <t>MatHang</t>
   </si>
@@ -864,18 +933,9 @@
     <t>LoaiHang</t>
   </si>
   <si>
-    <t>ChatLieu</t>
-  </si>
-  <si>
-    <t>MauSac</t>
-  </si>
-  <si>
     <t>TenLH</t>
   </si>
   <si>
-    <t>SoLuongTonKho</t>
-  </si>
-  <si>
     <t>TrangThaiDonHang</t>
   </si>
   <si>
@@ -885,27 +945,6 @@
     <t>PhuongThucThanhToan</t>
   </si>
   <si>
-    <t>NgayThanhToan</t>
-  </si>
-  <si>
-    <t>NgayTaoDonHang</t>
-  </si>
-  <si>
-    <t>NhanVienTaoDonHang</t>
-  </si>
-  <si>
-    <t>ThanhTien</t>
-  </si>
-  <si>
-    <t>NguoiDung</t>
-  </si>
-  <si>
-    <t>MaND</t>
-  </si>
-  <si>
-    <t>TenND</t>
-  </si>
-  <si>
     <t>SoDienThoai</t>
   </si>
   <si>
@@ -933,12 +972,6 @@
     <t>TenCV</t>
   </si>
   <si>
-    <t>ChucVuNguoiDung</t>
-  </si>
-  <si>
-    <t>PhieuNhap</t>
-  </si>
-  <si>
     <t>MaPN</t>
   </si>
   <si>
@@ -957,62 +990,77 @@
     <t>NhaCungCap</t>
   </si>
   <si>
-    <t>DiaChi</t>
-  </si>
-  <si>
-    <t>MaDC</t>
-  </si>
-  <si>
-    <t>GhiChu</t>
-  </si>
-  <si>
-    <t>NguoiDungDiaChi</t>
-  </si>
-  <si>
-    <t>MaMS</t>
-  </si>
-  <si>
-    <t>TenMS</t>
-  </si>
-  <si>
     <t>TinhTrangDon</t>
   </si>
   <si>
     <t>NhanVienPhuTrach</t>
   </si>
   <si>
-    <t>TaiKhoanMXH</t>
-  </si>
-  <si>
     <t>MaTK</t>
   </si>
   <si>
-    <t>MXH</t>
-  </si>
-  <si>
     <t>MaPTTT</t>
   </si>
   <si>
     <t>TenPTTT</t>
   </si>
   <si>
-    <t>KDL</t>
-  </si>
-  <si>
-    <t>DanhSach</t>
-  </si>
-  <si>
-    <t>DoiTuong</t>
-  </si>
-  <si>
-    <t>Xử lý</t>
+    <t>HinhAnh(s)</t>
+  </si>
+  <si>
+    <t>MauSac(s)</t>
+  </si>
+  <si>
+    <t>ChatLieu(s)</t>
+  </si>
+  <si>
+    <t>KichCo(s)</t>
+  </si>
+  <si>
+    <t>Đi kèm với</t>
+  </si>
+  <si>
+    <t>đơn vị kích cỡ</t>
+  </si>
+  <si>
+    <t>TenKH</t>
+  </si>
+  <si>
+    <t>MaNV</t>
+  </si>
+  <si>
+    <t>TenNV</t>
+  </si>
+  <si>
+    <t>TaiKhoan</t>
+  </si>
+  <si>
+    <t>TenTK</t>
+  </si>
+  <si>
+    <t>TongTien</t>
+  </si>
+  <si>
+    <t>ThongTinNhapHang</t>
+  </si>
+  <si>
+    <t>MAKC</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Lhn5nfSBxkdXNRi3eJmCdsIFWPohW5YO/view?usp=sharing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1098,6 +1146,43 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1215,10 +1300,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1372,12 +1458,17 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1704,11 +1795,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A4:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:K13"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,32 +1808,15 @@
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
-    <col min="13" max="14" width="21" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" customWidth="1"/>
-    <col min="17" max="22" width="12.7109375" customWidth="1"/>
+    <col min="5" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="18" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F2" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="48"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F3" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="48"/>
-    </row>
-    <row r="4" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1756,40 +1830,28 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>241</v>
+        <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>269</v>
+        <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="O4" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1799,91 +1861,70 @@
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
+      <c r="E5" s="59" t="s">
+        <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>242</v>
+        <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>251</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="59" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+      <c r="L6" s="59" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>258</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1895,174 +1936,152 @@
         <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>263</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>259</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>234</v>
+      <c r="D8" s="59" t="s">
+        <v>231</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+        <v>235</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="59" t="s">
         <v>229</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="G9" s="2"/>
+        <v>238</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>230</v>
+    </row>
+    <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="59" t="s">
+        <v>256</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>236</v>
+      <c r="D10" s="59" t="s">
+        <v>233</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="G10" s="2"/>
+        <v>237</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>237</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2" t="s">
-        <v>259</v>
+      <c r="J10" s="59" t="s">
+        <v>247</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>231</v>
+    </row>
+    <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="59" t="s">
+        <v>255</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>237</v>
+      <c r="D11" s="59" t="s">
+        <v>247</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G11" s="2"/>
+      <c r="F11" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="G11" s="59" t="s">
+        <v>240</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>5</v>
+    </row>
+    <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="59" t="s">
+        <v>254</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>238</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="H12" s="59"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-    </row>
-    <row r="13" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>233</v>
+        <v>17</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>239</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>250</v>
-      </c>
+      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -2074,12 +2093,8 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-    </row>
-    <row r="15" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2091,12 +2106,8 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-    </row>
-    <row r="16" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -2108,12 +2119,8 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -2125,12 +2132,8 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -2142,12 +2145,8 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -2159,12 +2158,8 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -2176,47 +2171,455 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="59" t="s">
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-    </row>
-    <row r="24" spans="2:16" s="18" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="18" t="s">
-        <v>274</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>277</v>
-      </c>
-      <c r="C25" t="s">
-        <v>276</v>
-      </c>
-    </row>
+    </row>
+    <row r="24" spans="2:12" s="18" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00967ACB-CFA1-460B-A734-E9F64BF353E8}">
+  <dimension ref="A4:L28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="18" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="59" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="L6" s="59" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>259</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="59" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="59" t="s">
+        <v>233</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="59" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="G11" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="59" t="s">
+        <v>254</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="H12" s="59"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" s="18" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="62" t="s">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B28" r:id="rId1" xr:uid="{4931FDE1-1D68-482A-986C-B027DF74A0DE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:U43"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O55" sqref="O55"/>
+    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2681,26 +3084,49 @@
       <c r="J26" s="8">
         <v>4</v>
       </c>
+      <c r="N26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="N27" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="O27" s="51" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>69</v>
       </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>70</v>
       </c>
-      <c r="N29" t="s">
-        <v>6</v>
-      </c>
-      <c r="R29" t="s">
-        <v>19</v>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>71</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
@@ -2711,6 +3137,12 @@
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
+      <c r="N31">
+        <v>2</v>
+      </c>
+      <c r="O31" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
@@ -2723,41 +3155,69 @@
       <c r="G32" s="23" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <v>2</v>
+      </c>
+      <c r="O32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>2</v>
+      </c>
+      <c r="O33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <v>3</v>
+      </c>
+      <c r="O34" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N35" s="60">
+        <v>2</v>
+      </c>
+      <c r="O35" s="60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="I36" s="48"/>
       <c r="J36" s="48"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
       <c r="I37" s="48"/>
       <c r="J37" s="48"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="I38" s="48"/>
       <c r="J38" s="48"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
       <c r="I39" s="48"/>
       <c r="J39" s="48"/>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="I40" s="48"/>
       <c r="J40" s="48"/>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
       <c r="I41" s="48"/>
       <c r="J41" s="48"/>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
       <c r="I42" s="52"/>
       <c r="J42" s="52"/>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
       <c r="I43" s="48"/>
       <c r="J43" s="48"/>
     </row>
@@ -2770,11 +3230,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:AJ77"/>
   <sheetViews>
-    <sheetView topLeftCell="S34" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="S16" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="Y48" sqref="Y48"/>
     </sheetView>
   </sheetViews>
@@ -4308,11 +4768,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
LESSON 16 - Database - 19.02.2025
</commit_message>
<xml_diff>
--- a/Java23 QuyenPhan Database Design.xlsx
+++ b/Java23 QuyenPhan Database Design.xlsx
@@ -8,21 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java23\3. Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349C1669-8412-4DF6-B078-A6A01BE6D247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4166D1C-5EF2-4C74-AFDB-4D5D11213092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="588" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="588" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
     <sheet name="B2. Mô hình logic" sheetId="5" r:id="rId2"/>
-    <sheet name="ERD - Mô hình logic" sheetId="2" r:id="rId3"/>
-    <sheet name="RD - Mô hình quan hệ" sheetId="3" r:id="rId4"/>
-    <sheet name="DB - Mô hình vật lý" sheetId="4" r:id="rId5"/>
+    <sheet name="B2. ERD - Mô hình logic" sheetId="2" r:id="rId3"/>
+    <sheet name="B3. Mô hình quan hệ" sheetId="6" r:id="rId4"/>
+    <sheet name="RD - Mô hình quan hệ" sheetId="3" r:id="rId5"/>
+    <sheet name="DB - Mô hình vật lý" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -68,7 +80,113 @@
     <author>Quyen Ngoc Phan</author>
   </authors>
   <commentList>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{F496D48F-A2BA-48FB-ACCA-2D383B7B2F89}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{830ABD6D-C41E-48FE-8DD6-80984A668707}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+GiaBan được xác định thông qua MatHang và KichCo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{F496D48F-A2BA-48FB-ACCA-2D383B7B2F89}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Lưu trữ cùng với kích cỡ, chất liệu, màu sắc</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{445A18A2-0EAE-4AC7-A7E2-01F758036FD1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Trong một phiếu có thể có nhiều nhà cung cấp</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Quyen Ngoc Phan</author>
+  </authors>
+  <commentList>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{74278309-1114-4129-B55F-D321AC11D33B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+GiaBan được xác định thông qua MatHang và KichCo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{7D63D11D-2A3D-4B2B-9F1A-67428B068415}">
       <text>
         <r>
           <rPr>
@@ -97,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="331">
   <si>
     <t>MatHang</t>
   </si>
@@ -1053,14 +1171,195 @@
     <t>XL</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/1Lhn5nfSBxkdXNRi3eJmCdsIFWPohW5YO/view?usp=sharing</t>
+    <t>ĐH1</t>
+  </si>
+  <si>
+    <t>MH A1</t>
+  </si>
+  <si>
+    <t>MH A2</t>
+  </si>
+  <si>
+    <t>MH A3</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>PhiGiaoHang</t>
+  </si>
+  <si>
+    <t>ĐH6</t>
+  </si>
+  <si>
+    <t>MH A4</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>NV1</t>
+  </si>
+  <si>
+    <t>Nhan Vien Giu Xe</t>
+  </si>
+  <si>
+    <t>NV2</t>
+  </si>
+  <si>
+    <t>Nguyen A</t>
+  </si>
+  <si>
+    <t>NV Giữ Xe</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>NV3</t>
+  </si>
+  <si>
+    <t>Le Nam</t>
+  </si>
+  <si>
+    <t>Nhân Viên Giữ Xe</t>
+  </si>
+  <si>
+    <t>Nhân Viên Bán Hàng</t>
+  </si>
+  <si>
+    <t>Nhân Viên Giao Hàng</t>
+  </si>
+  <si>
+    <t>Quản Lý Bán Hàng</t>
+  </si>
+  <si>
+    <t>Một số đối tượng dù chỉ có một thuộc tính thường là VARCHAR nhưng</t>
+  </si>
+  <si>
+    <t>vẫn nên tạo đối tượng để xem đối tượng đó như là ENUM để lưu</t>
+  </si>
+  <si>
+    <t>tập các hằng số sau đó dùng ở những đối tượng khác</t>
+  </si>
+  <si>
+    <t>Tránh dùng dữ liệu không đồng nhất</t>
+  </si>
+  <si>
+    <t>Ví dụ</t>
+  </si>
+  <si>
+    <t>PN1</t>
+  </si>
+  <si>
+    <t>ChiTietNhapHang</t>
+  </si>
+  <si>
+    <t>PN2</t>
+  </si>
+  <si>
+    <t>PN3</t>
+  </si>
+  <si>
+    <t>MaTTDH</t>
+  </si>
+  <si>
+    <t>Sự kết hợp giữa DonHang 
+và MatHang</t>
+  </si>
+  <si>
+    <t>PhieuNhapHang</t>
+  </si>
+  <si>
+    <t>MaNCC</t>
+  </si>
+  <si>
+    <t>TenNhaCC</t>
+  </si>
+  <si>
+    <t>MaSoThue</t>
+  </si>
+  <si>
+    <t>JAVA23 SHOPPING DIAGRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://viewer.diagrams.net/index.html?tags=%7B%7D&amp;lightbox=1&amp;highlight=0000ff&amp;edit=_blank&amp;layers=1&amp;nav=1&amp;title=java23%20shopping.drawio&amp;dark=auto#R%3Cmxfile%3E%3Cdiagram%20name%3D%22Page-1%22%20id%3D%22tJi9Ov7fiK_nzWUJrZYH%22%3E1Vxdd6I6FP01POoi4dPHip3pWp12dVa9M3eeZqWYCvcicRCq3l9%2FgwSEGBWRIO1LmwOJkLOzzz4nsYrmLDZfI7T0nsgMBwpUZxtFmygQQgPq9Fdq2TKLqjHLPPJnmQ3sDa%2F%2Bf5gZVWZN%2FBleVW6MCQlif1k1uiQMsRtXbCiKyLp62zsJqp%2B6RHN8YHh1UXBo%2FenPYi%2Bz2oa6tz9gf%2B7lnwxUdmWB8puZYeWhGVmXTNq9ojkRIXH212Lj4CCdvXxesn5fjlwtHizCYVynw79%2Fxd5Af9YWMwtFXx6XjjsdDNgoHyhI2Asr0AzoeON3QoelTx1v2VSYfxKSXxisdo66ozdAuKTeHu%2Bv07%2Fm6e8nFD%2BgcJ6PRx8sGzK7yuakGB3Sh6U%2BpY3x2vNj%2FLpEbnplTXFFbV68CGgLFD3L752%2FBI5ivCmZ2Dx8xWSB42hLb2FXLeYSBsoRa673Dga517ySc21mQwxT82Lg%2FbTTP9jMX%2BAFKM8Lj77rOaSPThgAzg3azf2gCfzAz1A4u0tphbbcAK1WvktnYxWjKD40l%2BYrIkk4w%2Blnq7RFJy3a%2Fp02hkbe%2FMXu3DUmm%2FKdk23e2vhx1k0HFmv%2FKl3bd0sb5V4vOPLpHOGI2Y76b0WSyMXnsUrfeI7j88yCZxV%2BPURDydmGwNe5LcIBiv2PKiuLAMA%2B4YX4u5WTRyKdw5rGYSh7b9arzKL8QKPqQAdgzCbmYKAdHovXbg5RXR5VfCPI7ytjD6BanfcBvDVZGA3J4jgrFKt7ZJQX99A%2BvbwLMilTSYlZTpBJe7Sgf0pa0DhUFbLzYlqA1YEAP1B7tHD%2Ftoz%2F%2Bf1z%2Ff335CleG%2B9%2F9NfvMnXchIQSWeGAAgTwO8oKJu8%2Bs0NSEPpBppLzkOv11hNa1RPGzT3RVMvVoOdrxVdT%2BSekzrN0fQqnZbo%2Bziu3YmfTrIJKtxqyswW4gWC37CxRtE0jyghTD%2Fl9pmn7kAygiAxGssigqVa7IrHTLa2qx0amVTO9A%2FXZJe0vFnGt0ERecTtHE%2FpNacLmVIDRkCZsHQxVa7T%2FqUo6FVIf7i%2FanVKIJY9Cnj0U%2FvBx2EfqKAqtvVF4I3mOePESkpJ54lJCD70pQb30iWYaVZ8I2D2%2FpeySojTeuk%2Fy8F5yyvPBFEUeWbwlq06miBccQDucI7tL1AJRgig1AhZi9qLCZu3I12KQs2oGOaCKfd5NlBtxGdYBVupGuREfLvlSqOxSxaEafv5B2y%2Becg%2BU8Vi5o9yhTiPF0ZQ74Hq0oTi6QrWhY1IDpUT1YXdNTdUuj2EKiG%2FoDQdVjKLAn4cpgCk4Up00Tle376Lgjl1Y%2BLNZOsY4wpSo0dtuvBRny3QadhNjjBVjcooe2BYk66wUvFjG5InFeZRM1CGwoVnxWZ6%2FXYkpUB1Vq%2FYn7%2B8rLAcCojJJS8l5uXQKTlJISaxrql0V66ptn6MsydJ7VJeVbklKOs8lTTN0g2e3jjN00H65SBgI65Xl024DCkLVLsfDoQ6N04A%2BWtHvNk7eEpEWlzDoZtNkkKst611X9EU1i5YSjQeCJqSfuQW%2FT9vlNp%2FYD%2BZFzBCSENerEDWjhUptaHiaD1pc%2Bzka%2B734DW4XTuczztrhiD%2BawpeUZC9%2BUblHSrrWAFYl3aTaXJETnsVxe7Lp1P5yv3GqcRsbjSuWJuSTQk7DS8ZprtquCFLAPhKkHM%2Bf%2Bji%2BdF%2FjUyaA1smgmEpBQ5OSAQ6AXR22sxwQiipSbW2KIf%2FR62n11OYOkN1%2BpzyPLW0pnKtCymWqqEWFA2sGjtseWLK5hFvnt0xrVwG5hFvXu1U48LKEu76sHhpW9VDFUAXaGRgJRYm4pNRZVRrWVTJHYkdHVWlecTeuSnOKW%2B%2B4Kp1%2FUUVGOHK8xP2R9DEYAf4MvuCkRsfBqP1jtVcW4ip7Ut1l3Dkg%2B73%2BgcofreLjSF0CACqXFGl8aJPNAKJCT2s7%2Bz5Onj207OsRLcBN%2Fv7LOWUmEG1ZSzuzBe3zTOAm0cduoWdr%2B%2FodoxrHrRpQSYu0ULcIn6H5ZlV4ThYMGp%2FctHhc1twYokhA29JtLI0%2FQWQj%2FpNY8fDoo%2FHvmD%2FaHvTZQ7TLUqLzR3XiY%2FffUZMtm6%2Bq%2F912fQAObI2%2FjcZtlwxqro7W6n%2FXF3HO1f8ujpqfsQCYreoTJ0BU3bA4T18HRPkFPk1UVmrvyKqThHOHKqEeiqmBzUcGXSCmRPQiTUxpovRWctgYqcWB99L3GOXtDZ3l%2FAyRN%2Bf8yzMjDk6tlUZoc%2F%2F%2FJ7Lb9%2F%2FGQ7v%2FHw%3D%3D%3C%2Fdiagram%3E%3C%2Fmxfile%3E#%7B%22pageId%22%3A%22tJi9Ov7fiK_nzWUJrZYH%22%7D </t>
+  </si>
+  <si>
+    <t>1. Xác định cấu trúc các bảng - TABLE</t>
+  </si>
+  <si>
+    <t>- Tập thực thể(B2) - Table</t>
+  </si>
+  <si>
+    <t>- Mối quan hệ(B2) NN - Table mới</t>
+  </si>
+  <si>
+    <t>2. Xác định các cột trong bảng - COLUMN NAME</t>
+  </si>
+  <si>
+    <t>- Thuộc tính(B2) - COLUMN</t>
+  </si>
+  <si>
+    <t>- Mối quan hệ(B2) 1N1 11 - COLUMN mới</t>
+  </si>
+  <si>
+    <t>3. Xác định khóa chính(PRIMARY KEY) cho từng TABLE</t>
+  </si>
+  <si>
+    <t>- B2 Xác định KHÓA cho tập thực thể, chọn ra KHÓA làm KHÓA CHÍNH để cài đặt cho TABLE trong csdl vật lý</t>
+  </si>
+  <si>
+    <t>- Đảm bảo bộ dữ liệu của khóa chính là không trùng nhau</t>
+  </si>
+  <si>
+    <t>4. Xác định khóa ngoại(FOREIGN KEY) của từng TABLE</t>
+  </si>
+  <si>
+    <t>- Khóa ngoại giúp tạo liên kết, ràng buộc giữa các Table trong csdl</t>
+  </si>
+  <si>
+    <t>MH4</t>
+  </si>
+  <si>
+    <t>Kẹo D</t>
+  </si>
+  <si>
+    <t>LH1</t>
+  </si>
+  <si>
+    <t>Bánh</t>
+  </si>
+  <si>
+    <t>LH2</t>
+  </si>
+  <si>
+    <t>Kẹo</t>
+  </si>
+  <si>
+    <t>LH3</t>
+  </si>
+  <si>
+    <t>Nước</t>
+  </si>
+  <si>
+    <t>- Quan hệ 1-n -&gt; Bỏ 1 vào nhiều -&gt; Tạo khóa ngoại ở bảng con(N) sau đó liên kết với khóa chính ở bảng cha(1)</t>
+  </si>
+  <si>
+    <t>- Lưu ý: Dữ liệu trong cột khóa ngoại có thể trùng nhau để đảm bảo mối liên kết 1-n</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1180,15 +1479,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1234,12 +1541,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1300,11 +1601,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1382,9 +1682,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1404,7 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1426,7 +1723,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1438,6 +1735,19 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1458,17 +1768,15 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1861,7 +2169,7 @@
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="53" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -1887,16 +2195,16 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="53" t="s">
         <v>257</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="53" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1917,7 +2225,7 @@
       <c r="K6" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="L6" s="59" t="s">
+      <c r="L6" s="53" t="s">
         <v>250</v>
       </c>
     </row>
@@ -1959,7 +2267,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="53" t="s">
         <v>231</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1982,7 +2290,7 @@
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="53" t="s">
         <v>229</v>
       </c>
       <c r="C9" s="2"/>
@@ -2005,11 +2313,11 @@
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="53" t="s">
         <v>256</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="53" t="s">
         <v>233</v>
       </c>
       <c r="E10" s="2"/>
@@ -2021,25 +2329,25 @@
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="59" t="s">
+      <c r="J10" s="53" t="s">
         <v>247</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="53" t="s">
         <v>255</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="53" t="s">
         <v>247</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="59" t="s">
+      <c r="F11" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="53" t="s">
         <v>240</v>
       </c>
       <c r="H11" s="2"/>
@@ -2051,17 +2359,17 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="53" t="s">
         <v>254</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="H12" s="59"/>
+      <c r="H12" s="53"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -2187,27 +2495,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00967ACB-CFA1-460B-A734-E9F64BF353E8}">
-  <dimension ref="A4:L28"/>
+  <dimension ref="A2:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="8" width="16.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="18" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="13" width="18.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="17" max="21" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F2" s="18" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2218,101 +2532,128 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="K4" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="61" t="s">
+    <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="59" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="55" t="s">
         <v>261</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="55" t="s">
         <v>251</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="55" t="s">
         <v>241</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="55" t="s">
         <v>243</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="55" t="s">
+        <v>243</v>
+      </c>
+      <c r="M5" s="55" t="s">
+        <v>305</v>
+      </c>
+      <c r="N5" s="55" t="s">
         <v>252</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="59" t="s">
+      <c r="O5" s="55" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="53" t="s">
         <v>257</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="M6" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="L6" s="59" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>258</v>
       </c>
@@ -2324,155 +2665,176 @@
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>234</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="2"/>
+      <c r="K7" s="53" t="s">
+        <v>247</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>259</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
+      <c r="B8" s="53" t="s">
+        <v>229</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>235</v>
-      </c>
+      <c r="E8" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
         <v>235</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>245</v>
-      </c>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="59" t="s">
-        <v>229</v>
+      <c r="L8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="53" t="s">
+        <v>256</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>232</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>238</v>
-      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>246</v>
-      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="59" t="s">
-        <v>256</v>
+      <c r="L9" s="53" t="s">
+        <v>248</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="53" t="s">
+        <v>255</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="53" t="s">
         <v>233</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
-        <v>237</v>
-      </c>
+      <c r="E10" s="53"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>237</v>
+      </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="59" t="s">
+      <c r="J10" s="2"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="53" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="53" t="s">
         <v>247</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="59" t="s">
-        <v>255</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="59" t="s">
-        <v>247</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="59" t="s">
+      <c r="E11" s="53"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="H11" s="53" t="s">
         <v>240</v>
       </c>
-      <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
-        <v>248</v>
-      </c>
+      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="59" t="s">
-        <v>254</v>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="2"/>
+      <c r="H12" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="H12" s="59"/>
-      <c r="I12" s="2"/>
+      <c r="I12" s="53"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="H13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -2484,8 +2846,11 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2497,8 +2862,11 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -2510,8 +2878,11 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -2523,8 +2894,11 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -2536,8 +2910,11 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -2549,8 +2926,11 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -2562,55 +2942,554 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" s="18" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" s="18" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24"/>
       <c r="C24" t="s">
         <v>71</v>
       </c>
       <c r="D24"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E24"/>
+      <c r="H24" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N24" s="53" t="s">
+        <v>261</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
         <v>72</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E25" s="9"/>
+      <c r="G25" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="H25" s="47" t="s">
+        <v>270</v>
+      </c>
+      <c r="I25" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="J25" s="47">
+        <v>2</v>
+      </c>
+      <c r="N25" s="47" t="s">
+        <v>281</v>
+      </c>
+      <c r="O25" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="P25" s="47" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
         <v>73</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E26" s="9"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="47" t="s">
+        <v>270</v>
+      </c>
+      <c r="I26" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="J26" s="47">
+        <v>4</v>
+      </c>
+      <c r="N26" s="47" t="s">
+        <v>283</v>
+      </c>
+      <c r="O26" s="47" t="s">
+        <v>284</v>
+      </c>
+      <c r="P26" s="47" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="62" t="s">
+      <c r="G27" s="56"/>
+      <c r="H27" s="47" t="s">
         <v>270</v>
       </c>
+      <c r="I27" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="J27" s="47">
+        <v>1</v>
+      </c>
+      <c r="N27" s="47" t="s">
+        <v>287</v>
+      </c>
+      <c r="O27" s="47" t="s">
+        <v>288</v>
+      </c>
+      <c r="P27" s="47" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H28" s="47" t="s">
+        <v>278</v>
+      </c>
+      <c r="I28" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="J28" s="47">
+        <v>2</v>
+      </c>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="47"/>
+      <c r="P28" s="47"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H29" s="47" t="s">
+        <v>278</v>
+      </c>
+      <c r="I29" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="J29" s="47">
+        <v>4</v>
+      </c>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
+      <c r="P29" s="47"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G30" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="H30" s="51" t="s">
+        <v>270</v>
+      </c>
+      <c r="I30" s="51" t="s">
+        <v>271</v>
+      </c>
+      <c r="J30" s="47">
+        <v>8</v>
+      </c>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="47"/>
+      <c r="P30" s="47"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N31" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="O31" s="47"/>
+      <c r="P31" s="47"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N32" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N33" s="5">
+        <v>1</v>
+      </c>
+      <c r="O33" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>0</v>
+      </c>
+      <c r="N34" s="5">
+        <v>2</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H35" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N35" s="5">
+        <v>3</v>
+      </c>
+      <c r="O35" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H36" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="J36" s="5">
+        <v>100</v>
+      </c>
+      <c r="N36" s="5">
+        <v>4</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H37" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="J37" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H38" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="J38" s="5">
+        <v>220</v>
+      </c>
+      <c r="N38" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="47"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="N39" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="47"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="N40" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="N41" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="47"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="N42" s="50" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="N43" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G44" s="47"/>
+      <c r="N44" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="C45" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D45" s="47">
+        <v>200</v>
+      </c>
+      <c r="E45" s="47">
+        <v>15</v>
+      </c>
+      <c r="F45" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="G45" s="47"/>
+      <c r="N45" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B46" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="C46" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="D46" s="47">
+        <v>120</v>
+      </c>
+      <c r="E46" s="47">
+        <v>12</v>
+      </c>
+      <c r="F46" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="G46" s="47"/>
+      <c r="N46" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="D47" s="47">
+        <v>400</v>
+      </c>
+      <c r="E47" s="47">
+        <v>10</v>
+      </c>
+      <c r="F47" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47" s="47"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="47"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="47"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="47"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="47" t="s">
+        <v>266</v>
+      </c>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="47"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D51" s="53" t="s">
+        <v>247</v>
+      </c>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="47"/>
+      <c r="H51" s="47"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="C52" s="52">
+        <v>18.02</v>
+      </c>
+      <c r="D52" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="47"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="47" t="s">
+        <v>300</v>
+      </c>
+      <c r="C53" s="52">
+        <v>18.02</v>
+      </c>
+      <c r="D53" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="47"/>
+      <c r="H53" s="47"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="C54" s="47">
+        <v>19.02</v>
+      </c>
+      <c r="D54" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54" s="47"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="47"/>
+      <c r="H54" s="47"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="47"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="47"/>
+      <c r="H55" s="47"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="47"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="47"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="47"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="47"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="47"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B28" r:id="rId1" xr:uid="{4931FDE1-1D68-482A-986C-B027DF74A0DE}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2619,7 +3498,7 @@
   <dimension ref="A2:U43"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:D33"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2638,7 +3517,7 @@
       <c r="L2" t="s">
         <v>224</v>
       </c>
-      <c r="M2" s="50"/>
+      <c r="M2" s="49"/>
       <c r="N2" s="23"/>
       <c r="O2" t="s">
         <v>153</v>
@@ -2659,10 +3538,10 @@
       <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="P4" s="51"/>
+      <c r="P4" s="50"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="N5" s="51"/>
+      <c r="N5" s="50"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -2853,12 +3732,12 @@
       <c r="Q13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="R13" s="53" t="s">
+      <c r="R13" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="S13" s="53"/>
-      <c r="T13" s="53"/>
-      <c r="U13" s="53"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="57"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D14" s="5"/>
@@ -2871,10 +3750,10 @@
       <c r="Q14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="R14" s="53"/>
-      <c r="S14" s="53"/>
-      <c r="T14" s="53"/>
-      <c r="U14" s="53"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="57"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
@@ -2882,7 +3761,7 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="J16" s="51"/>
+      <c r="J16" s="50"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
@@ -3089,10 +3968,10 @@
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="N27" s="51" t="s">
+      <c r="N27" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="O27" s="51" t="s">
+      <c r="O27" s="50" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3162,7 +4041,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>74</v>
       </c>
@@ -3173,7 +4052,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="N34">
         <v>3</v>
       </c>
@@ -3181,45 +4060,53 @@
         <v>269</v>
       </c>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="N35" s="60">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>308</v>
+      </c>
+      <c r="G35" s="56"/>
+      <c r="N35" s="54">
         <v>2</v>
       </c>
-      <c r="O35" s="60" t="s">
+      <c r="O35" s="54" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
-    </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
-    </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
-    </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
-    </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I40" s="48"/>
-      <c r="J40" s="48"/>
-    </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
-    </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I42" s="52"/>
-      <c r="J42" s="52"/>
-    </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>309</v>
+      </c>
+      <c r="G36" s="56"/>
+      <c r="I36" s="47"/>
+      <c r="J36" s="47"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I37" s="47"/>
+      <c r="J37" s="47"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I38" s="47"/>
+      <c r="J38" s="47"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I39" s="47"/>
+      <c r="J39" s="47"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I40" s="47"/>
+      <c r="J40" s="47"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I42" s="51"/>
+      <c r="J42" s="51"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3231,11 +4118,662 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD2C7DF-5616-418E-B427-D50946AF144B}">
+  <dimension ref="A2:Q58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="13" width="18.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="17" max="21" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F2" s="18" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="55" t="s">
+        <v>261</v>
+      </c>
+      <c r="I5" s="55" t="s">
+        <v>251</v>
+      </c>
+      <c r="J5" s="55" t="s">
+        <v>241</v>
+      </c>
+      <c r="K5" s="55" t="s">
+        <v>243</v>
+      </c>
+      <c r="L5" s="55" t="s">
+        <v>243</v>
+      </c>
+      <c r="M5" s="55" t="s">
+        <v>305</v>
+      </c>
+      <c r="N5" s="55" t="s">
+        <v>252</v>
+      </c>
+      <c r="O5" s="55" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="53" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L6" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="53" t="s">
+        <v>247</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>259</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="53" t="s">
+        <v>231</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="53" t="s">
+        <v>256</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="53" t="s">
+        <v>248</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="53" t="s">
+        <v>255</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="53" t="s">
+        <v>233</v>
+      </c>
+      <c r="E10" s="53"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="53" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="53" t="s">
+        <v>247</v>
+      </c>
+      <c r="E11" s="53"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="53" t="s">
+        <v>263</v>
+      </c>
+      <c r="H11" s="53" t="s">
+        <v>240</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="53" t="s">
+        <v>263</v>
+      </c>
+      <c r="I12" s="53"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C23" s="63" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="C24" s="23" t="s">
+        <v>311</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C25" s="23" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C27" s="63" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C28" s="23" t="s">
+        <v>314</v>
+      </c>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="47"/>
+      <c r="P28" s="47"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C29" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
+      <c r="P29" s="47"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="47"/>
+      <c r="P30" s="47"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C31" s="63" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C32" s="23" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="23" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="63" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="23" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="23"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="23" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="47"/>
+      <c r="C39" s="65" t="s">
+        <v>330</v>
+      </c>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="47"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="47"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F51" s="47"/>
+      <c r="G51" s="47"/>
+      <c r="H51" s="47"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="47"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F53" s="47"/>
+      <c r="G53" s="47"/>
+      <c r="H53" s="47"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F54" s="47"/>
+      <c r="G54" s="47"/>
+      <c r="H54" s="47"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="47"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="47"/>
+      <c r="H55" s="47"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="47"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="47"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="47"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="47"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="47"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:AJ77"/>
   <sheetViews>
-    <sheetView topLeftCell="S16" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="Y48" sqref="Y48"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3474,6 +5012,15 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B14" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>229</v>
+      </c>
       <c r="P14" s="4" t="s">
         <v>86</v>
       </c>
@@ -3486,11 +5033,47 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="64" t="s">
+        <v>229</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="T15" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="4">
+        <v>20</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>324</v>
+      </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
@@ -3502,7 +5085,45 @@
       <c r="X16" s="9"/>
       <c r="Y16" s="9"/>
     </row>
-    <row r="18" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="4">
+        <v>30</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="18" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="4">
+        <v>60</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>328</v>
+      </c>
       <c r="T18" s="21" t="s">
         <v>103</v>
       </c>
@@ -3510,11 +5131,23 @@
       <c r="V18" s="20"/>
       <c r="W18" s="5"/>
     </row>
-    <row r="19" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="P19" s="58" t="s">
+    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="D19" s="4">
+        <v>60</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="P19" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="Q19" s="58"/>
+      <c r="Q19" s="62"/>
       <c r="T19" s="4" t="s">
         <v>9</v>
       </c>
@@ -3528,14 +5161,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:35" x14ac:dyDescent="0.25">
       <c r="P20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Q20" s="57" t="s">
+      <c r="Q20" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="R20" s="57"/>
+      <c r="R20" s="61"/>
       <c r="T20" s="4" t="s">
         <v>94</v>
       </c>
@@ -3549,14 +5182,14 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
       <c r="P21" s="4">
         <v>1</v>
       </c>
-      <c r="Q21" s="57" t="s">
+      <c r="Q21" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="R21" s="57"/>
+      <c r="R21" s="61"/>
       <c r="T21" s="4" t="s">
         <v>94</v>
       </c>
@@ -3570,14 +5203,17 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>212</v>
+      </c>
       <c r="P22" s="4">
         <v>2</v>
       </c>
-      <c r="Q22" s="57" t="s">
+      <c r="Q22" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="R22" s="57"/>
+      <c r="R22" s="61"/>
       <c r="T22" s="4" t="s">
         <v>94</v>
       </c>
@@ -3591,14 +5227,20 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="D23" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>67</v>
+      </c>
       <c r="P23" s="4">
         <v>3</v>
       </c>
-      <c r="Q23" s="57" t="s">
+      <c r="Q23" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="R23" s="57"/>
+      <c r="R23" s="61"/>
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
@@ -3613,14 +5255,22 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="K24" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
       <c r="P24" s="4">
         <v>4</v>
       </c>
-      <c r="Q24" s="57" t="s">
+      <c r="Q24" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="R24" s="57"/>
+      <c r="R24" s="61"/>
       <c r="T24" s="4" t="s">
         <v>95</v>
       </c>
@@ -3640,7 +5290,39 @@
         <v>215</v>
       </c>
     </row>
-    <row r="28" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="D25" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="J25" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="K25" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="L25" s="35"/>
+      <c r="M25" s="33"/>
+    </row>
+    <row r="26" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="D26" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J26" s="31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="D27" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="J27" s="31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="T28" s="21" t="s">
         <v>155</v>
       </c>
@@ -3652,33 +5334,27 @@
       <c r="AA28" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AD28" s="46" t="s">
+      <c r="AD28" s="45" t="s">
         <v>93</v>
       </c>
       <c r="AF28" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C29" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="F29" t="s">
-        <v>212</v>
-      </c>
       <c r="H29" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="J29" s="30" t="s">
-        <v>67</v>
-      </c>
       <c r="P29" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="T29" s="39" t="s">
+      <c r="T29" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="U29" s="39" t="s">
+      <c r="U29" s="38" t="s">
         <v>121</v>
       </c>
       <c r="V29" s="28" t="s">
@@ -3690,7 +5366,7 @@
       <c r="Y29" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AA29" s="42" t="s">
+      <c r="AA29" s="41" t="s">
         <v>20</v>
       </c>
       <c r="AB29" s="4" t="s">
@@ -3699,10 +5375,10 @@
       <c r="AC29" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="AD29" s="44" t="s">
+      <c r="AD29" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="AF29" s="42" t="s">
+      <c r="AF29" s="41" t="s">
         <v>9</v>
       </c>
       <c r="AG29" s="4" t="s">
@@ -3711,18 +5387,18 @@
       <c r="AH29" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="AI29" s="42" t="s">
+      <c r="AI29" s="41" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C30" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D30" s="47" t="s">
+      <c r="D30" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="E30" s="47" t="s">
+      <c r="E30" s="46" t="s">
         <v>124</v>
       </c>
       <c r="F30" s="25" t="s">
@@ -3731,17 +5407,9 @@
       <c r="H30" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I30" s="47" t="s">
+      <c r="I30" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J30" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="K30" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="L30" s="34"/>
-      <c r="M30" s="34"/>
       <c r="P30" s="6" t="s">
         <v>122</v>
       </c>
@@ -3766,58 +5434,50 @@
       <c r="Y30" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="AA30" s="43" t="s">
+      <c r="AA30" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="AB30" s="41" t="s">
+      <c r="AB30" s="40" t="s">
         <v>192</v>
       </c>
       <c r="AC30" s="4">
         <v>225</v>
       </c>
-      <c r="AD30" s="43" t="s">
+      <c r="AD30" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="AF30" s="43" t="s">
+      <c r="AF30" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="AG30" s="41" t="s">
+      <c r="AG30" s="40" t="s">
         <v>196</v>
       </c>
       <c r="AH30" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="AI30" s="43" t="s">
+      <c r="AI30" s="42" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="C31" s="47" t="s">
+    <row r="31" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="C31" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="D31" s="47" t="s">
+      <c r="D31" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="47">
+      <c r="E31" s="46">
         <v>8</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H31" s="47" t="s">
+      <c r="H31" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="I31" s="47" t="s">
+      <c r="I31" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="J31" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="K31" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="L31" s="36"/>
-      <c r="M31" s="34"/>
       <c r="P31" s="4" t="s">
         <v>125</v>
       </c>
@@ -3842,52 +5502,49 @@
       <c r="Y31" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="AA31" s="43" t="s">
+      <c r="AA31" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="AB31" s="41" t="s">
+      <c r="AB31" s="40" t="s">
         <v>193</v>
       </c>
       <c r="AC31" s="4">
         <v>0</v>
       </c>
-      <c r="AD31" s="43" t="s">
+      <c r="AD31" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="AF31" s="43" t="s">
+      <c r="AF31" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="AG31" s="41" t="s">
+      <c r="AG31" s="40" t="s">
         <v>197</v>
       </c>
       <c r="AH31" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="AI31" s="43" t="s">
+      <c r="AI31" s="42" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="C32" s="47" t="s">
+    <row r="32" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="C32" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="D32" s="47" t="s">
+      <c r="D32" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="47">
+      <c r="E32" s="46">
         <v>6</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H32" s="47" t="s">
+      <c r="H32" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="I32" s="47" t="s">
+      <c r="I32" s="46" t="s">
         <v>134</v>
-      </c>
-      <c r="J32" s="32" t="s">
-        <v>126</v>
       </c>
       <c r="P32" s="4" t="s">
         <v>126</v>
@@ -3913,52 +5570,49 @@
       <c r="Y32" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="AA32" s="43" t="s">
+      <c r="AA32" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="AB32" s="41" t="s">
+      <c r="AB32" s="40" t="s">
         <v>194</v>
       </c>
       <c r="AC32" s="4">
         <v>125</v>
       </c>
-      <c r="AD32" s="43" t="s">
+      <c r="AD32" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="AF32" s="43" t="s">
+      <c r="AF32" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="AG32" s="41" t="s">
+      <c r="AG32" s="40" t="s">
         <v>198</v>
       </c>
       <c r="AH32" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="AI32" s="43" t="s">
+      <c r="AI32" s="42" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="33" spans="3:36" x14ac:dyDescent="0.25">
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="D33" s="47" t="s">
+      <c r="D33" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="47">
+      <c r="E33" s="46">
         <v>9</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H33" s="47" t="s">
+      <c r="H33" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="I33" s="47" t="s">
+      <c r="I33" s="46" t="s">
         <v>135</v>
-      </c>
-      <c r="J33" s="32" t="s">
-        <v>125</v>
       </c>
       <c r="P33" s="4" t="s">
         <v>127</v>
@@ -3978,39 +5632,39 @@
       <c r="V33" s="28">
         <v>5</v>
       </c>
-      <c r="AA33" s="43" t="s">
+      <c r="AA33" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="AB33" s="41" t="s">
+      <c r="AB33" s="40" t="s">
         <v>195</v>
       </c>
       <c r="AC33" s="4">
         <v>220</v>
       </c>
-      <c r="AD33" s="43" t="s">
+      <c r="AD33" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="AF33" s="43" t="s">
+      <c r="AF33" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="AG33" s="41" t="s">
+      <c r="AG33" s="40" t="s">
         <v>198</v>
       </c>
       <c r="AH33" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="AI33" s="43" t="s">
+      <c r="AI33" s="42" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="34" spans="3:36" x14ac:dyDescent="0.25">
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="D34" s="47" t="s">
+      <c r="D34" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="E34" s="47">
+      <c r="E34" s="46">
         <v>7</v>
       </c>
       <c r="F34" s="8" t="s">
@@ -4025,10 +5679,10 @@
       <c r="R34" s="3">
         <v>2</v>
       </c>
-      <c r="T34" s="37" t="s">
+      <c r="T34" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="U34" s="37" t="s">
+      <c r="U34" s="36" t="s">
         <v>126</v>
       </c>
       <c r="V34" s="28">
@@ -4036,13 +5690,13 @@
       </c>
     </row>
     <row r="35" spans="3:36" x14ac:dyDescent="0.25">
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="47" t="s">
+      <c r="D35" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="E35" s="47">
+      <c r="E35" s="46">
         <v>7</v>
       </c>
       <c r="F35" s="4" t="s">
@@ -4059,7 +5713,7 @@
       </c>
     </row>
     <row r="37" spans="3:36" x14ac:dyDescent="0.25">
-      <c r="C37" s="33" t="s">
+      <c r="C37" s="32" t="s">
         <v>151</v>
       </c>
       <c r="D37" s="9"/>
@@ -4071,7 +5725,7 @@
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
-      <c r="P37" s="33" t="s">
+      <c r="P37" s="32" t="s">
         <v>211</v>
       </c>
       <c r="Q37" s="9"/>
@@ -4130,7 +5784,7 @@
       <c r="C41" t="s">
         <v>136</v>
       </c>
-      <c r="AA41" s="49" t="s">
+      <c r="AA41" s="48" t="s">
         <v>145</v>
       </c>
     </row>
@@ -4138,16 +5792,16 @@
       <c r="C42" t="s">
         <v>139</v>
       </c>
-      <c r="AA42" s="45" t="s">
+      <c r="AA42" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="AB42" s="45"/>
-      <c r="AC42" s="45"/>
-      <c r="AD42" s="45"/>
-      <c r="AE42" s="45"/>
-      <c r="AF42" s="45"/>
-      <c r="AG42" s="45"/>
-      <c r="AH42" s="45"/>
+      <c r="AB42" s="44"/>
+      <c r="AC42" s="44"/>
+      <c r="AD42" s="44"/>
+      <c r="AE42" s="44"/>
+      <c r="AF42" s="44"/>
+      <c r="AG42" s="44"/>
+      <c r="AH42" s="44"/>
     </row>
     <row r="43" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
@@ -4172,7 +5826,7 @@
       <c r="C45" t="s">
         <v>141</v>
       </c>
-      <c r="O45" s="38" t="s">
+      <c r="O45" s="37" t="s">
         <v>7</v>
       </c>
       <c r="P45" s="28" t="s">
@@ -4210,10 +5864,10 @@
       <c r="P46" s="28">
         <v>1</v>
       </c>
-      <c r="Q46" s="40" t="s">
+      <c r="Q46" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="R46" s="40" t="s">
+      <c r="R46" s="39" t="s">
         <v>163</v>
       </c>
       <c r="T46" s="28" t="s">
@@ -4242,10 +5896,10 @@
       <c r="P47" s="28">
         <v>2</v>
       </c>
-      <c r="Q47" s="40" t="s">
+      <c r="Q47" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="R47" s="40" t="s">
+      <c r="R47" s="39" t="s">
         <v>177</v>
       </c>
       <c r="T47" s="28" t="s">
@@ -4265,26 +5919,26 @@
       </c>
     </row>
     <row r="48" spans="3:36" x14ac:dyDescent="0.25">
-      <c r="C48" s="54" t="s">
+      <c r="C48" s="58" t="s">
         <v>220</v>
       </c>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="55"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="59"/>
+      <c r="H48" s="59"/>
+      <c r="I48" s="59"/>
+      <c r="J48" s="59"/>
       <c r="O48" s="28">
         <v>3</v>
       </c>
       <c r="P48" s="28">
         <v>3</v>
       </c>
-      <c r="Q48" s="40" t="s">
+      <c r="Q48" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="R48" s="40" t="s">
+      <c r="R48" s="39" t="s">
         <v>172</v>
       </c>
       <c r="T48" s="28" t="s">
@@ -4296,34 +5950,34 @@
       <c r="V48" s="28">
         <v>9</v>
       </c>
-      <c r="AE48" s="42" t="s">
+      <c r="AE48" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="AF48" s="43" t="s">
+      <c r="AF48" s="42" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" spans="3:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="56" t="s">
+      <c r="C49" s="60" t="s">
         <v>219</v>
       </c>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="56"/>
-      <c r="I49" s="56"/>
-      <c r="J49" s="56"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="60"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="60"/>
+      <c r="J49" s="60"/>
       <c r="O49" s="28">
         <v>4</v>
       </c>
       <c r="P49" s="28">
         <v>4</v>
       </c>
-      <c r="Q49" s="40" t="s">
+      <c r="Q49" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="R49" s="40" t="s">
+      <c r="R49" s="39" t="s">
         <v>178</v>
       </c>
       <c r="T49" s="28" t="s">
@@ -4335,10 +5989,10 @@
       <c r="V49" s="28">
         <v>9</v>
       </c>
-      <c r="AE49" s="43" t="s">
+      <c r="AE49" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="AF49" s="43" t="s">
+      <c r="AF49" s="42" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4349,16 +6003,16 @@
       <c r="P50" s="28">
         <v>5</v>
       </c>
-      <c r="Q50" s="40" t="s">
+      <c r="Q50" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="R50" s="40" t="s">
+      <c r="R50" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="AE50" s="43" t="s">
+      <c r="AE50" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="AF50" s="43" t="s">
+      <c r="AF50" s="42" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4369,16 +6023,16 @@
       <c r="P51" s="28">
         <v>6</v>
       </c>
-      <c r="Q51" s="40" t="s">
+      <c r="Q51" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="R51" s="40" t="s">
+      <c r="R51" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="AE51" s="43" t="s">
+      <c r="AE51" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="AF51" s="43" t="s">
+      <c r="AF51" s="42" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4395,16 +6049,16 @@
       <c r="P52" s="28">
         <v>7</v>
       </c>
-      <c r="Q52" s="40" t="s">
+      <c r="Q52" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="R52" s="40" t="s">
+      <c r="R52" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="AE52" s="43" t="s">
+      <c r="AE52" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="AF52" s="43" t="s">
+      <c r="AF52" s="42" t="s">
         <v>202</v>
       </c>
     </row>
@@ -4412,10 +6066,10 @@
       <c r="C53" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D53" s="47" t="s">
+      <c r="D53" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="E53" s="47" t="s">
+      <c r="E53" s="46" t="s">
         <v>124</v>
       </c>
       <c r="F53" t="s">
@@ -4424,7 +6078,7 @@
       <c r="H53" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I53" s="47" t="s">
+      <c r="I53" s="46" t="s">
         <v>39</v>
       </c>
       <c r="J53" t="s">
@@ -4436,58 +6090,58 @@
       <c r="P53" s="28">
         <v>8</v>
       </c>
-      <c r="Q53" s="40" t="s">
+      <c r="Q53" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="R53" s="40" t="s">
+      <c r="R53" s="39" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="54" spans="3:32" x14ac:dyDescent="0.25">
-      <c r="C54" s="47" t="s">
+      <c r="C54" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="D54" s="47" t="s">
+      <c r="D54" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E54" s="47">
+      <c r="E54" s="46">
         <v>8</v>
       </c>
       <c r="F54" t="s">
         <v>130</v>
       </c>
-      <c r="H54" s="47"/>
-      <c r="I54" s="47"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
       <c r="O54" s="28">
         <v>9</v>
       </c>
       <c r="P54" s="28">
         <v>1</v>
       </c>
-      <c r="Q54" s="40" t="s">
+      <c r="Q54" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="R54" s="40" t="s">
+      <c r="R54" s="39" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="55" spans="3:32" x14ac:dyDescent="0.25">
-      <c r="C55" s="47" t="s">
+      <c r="C55" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="D55" s="47" t="s">
+      <c r="D55" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="E55" s="47">
+      <c r="E55" s="46">
         <v>6</v>
       </c>
       <c r="F55" t="s">
         <v>130</v>
       </c>
-      <c r="H55" s="47" t="s">
+      <c r="H55" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="I55" s="47" t="s">
+      <c r="I55" s="46" t="s">
         <v>134</v>
       </c>
       <c r="J55" t="s">
@@ -4502,30 +6156,30 @@
       <c r="P55" s="28">
         <v>2</v>
       </c>
-      <c r="Q55" s="40" t="s">
+      <c r="Q55" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="R55" s="40" t="s">
+      <c r="R55" s="39" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="56" spans="3:32" x14ac:dyDescent="0.25">
-      <c r="C56" s="47" t="s">
+      <c r="C56" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="D56" s="47" t="s">
+      <c r="D56" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="E56" s="47">
+      <c r="E56" s="46">
         <v>9</v>
       </c>
       <c r="F56" t="s">
         <v>132</v>
       </c>
-      <c r="H56" s="47" t="s">
+      <c r="H56" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="I56" s="47" t="s">
+      <c r="I56" s="46" t="s">
         <v>135</v>
       </c>
       <c r="J56" t="s">
@@ -4537,21 +6191,21 @@
       <c r="P56" s="28">
         <v>3</v>
       </c>
-      <c r="Q56" s="40" t="s">
+      <c r="Q56" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="R56" s="40" t="s">
+      <c r="R56" s="39" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="57" spans="3:32" x14ac:dyDescent="0.25">
-      <c r="C57" s="47" t="s">
+      <c r="C57" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="D57" s="47" t="s">
+      <c r="D57" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="E57" s="47">
+      <c r="E57" s="46">
         <v>7</v>
       </c>
       <c r="F57" t="s">
@@ -4563,21 +6217,21 @@
       <c r="P57" s="28">
         <v>4</v>
       </c>
-      <c r="Q57" s="40" t="s">
+      <c r="Q57" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="R57" s="40" t="s">
+      <c r="R57" s="39" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="58" spans="3:32" x14ac:dyDescent="0.25">
-      <c r="C58" s="47" t="s">
+      <c r="C58" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="D58" s="47" t="s">
+      <c r="D58" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="E58" s="47">
+      <c r="E58" s="46">
         <v>7</v>
       </c>
       <c r="F58" t="s">
@@ -4589,10 +6243,10 @@
       <c r="P58" s="28">
         <v>5</v>
       </c>
-      <c r="Q58" s="40" t="s">
+      <c r="Q58" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="R58" s="40" t="s">
+      <c r="R58" s="39" t="s">
         <v>184</v>
       </c>
     </row>
@@ -4603,10 +6257,10 @@
       <c r="P59" s="28">
         <v>6</v>
       </c>
-      <c r="Q59" s="40" t="s">
+      <c r="Q59" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="R59" s="40" t="s">
+      <c r="R59" s="39" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4617,10 +6271,10 @@
       <c r="P60" s="28">
         <v>7</v>
       </c>
-      <c r="Q60" s="40" t="s">
+      <c r="Q60" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="R60" s="40" t="s">
+      <c r="R60" s="39" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4631,10 +6285,10 @@
       <c r="P61" s="28">
         <v>8</v>
       </c>
-      <c r="Q61" s="40" t="s">
+      <c r="Q61" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="R61" s="40" t="s">
+      <c r="R61" s="39" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4768,7 +6422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:N26"/>
   <sheetViews>

</xml_diff>